<commit_message>
Revision no conformidades organizacionales
</commit_message>
<xml_diff>
--- a/Proyectos/2016/Calidad/No_conformidades_organizacionales.xlsx
+++ b/Proyectos/2016/Calidad/No_conformidades_organizacionales.xlsx
@@ -47,7 +47,7 @@
     <t>Jovanny zepeda</t>
   </si>
   <si>
-    <t>En proceso</t>
+    <t>Cerrada</t>
   </si>
 </sst>
 </file>
@@ -292,7 +292,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -364,7 +364,9 @@
       <c r="D4" s="5" t="n">
         <v>42433</v>
       </c>
-      <c r="E4" s="5"/>
+      <c r="E4" s="5" t="n">
+        <v>42433</v>
+      </c>
       <c r="F4" s="6" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Auditoría de seguimiento a actividades (Compras y Ventas) del 24/mar al 31/mar
</commit_message>
<xml_diff>
--- a/Proyectos/2016/Calidad/No_conformidades_organizacionales.xlsx
+++ b/Proyectos/2016/Calidad/No_conformidades_organizacionales.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="No Conformidades" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0" iterate="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="23">
   <si>
     <t>REPORTE DE NO CONFORMIDADES</t>
   </si>
@@ -77,6 +77,18 @@
   </si>
   <si>
     <t>Compras</t>
+  </si>
+  <si>
+    <t>Algunas de las actividades de ventas no tienen comentarios de seguimiento.</t>
+  </si>
+  <si>
+    <t>Hizo falta cronometrar varias tareas.</t>
+  </si>
+  <si>
+    <t>Hay muchas tareas que no estan cerradas a tiempo y no fueron reagendadas ni tienen comentario.</t>
+  </si>
+  <si>
+    <t>Solo una tarea no tenia registrado el tiempo.</t>
   </si>
 </sst>
 </file>
@@ -179,50 +191,50 @@
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -574,398 +586,446 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:G2"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="8"/>
-    <col min="2" max="2" width="42" style="15"/>
-    <col min="3" max="3" width="18.7109375" style="8"/>
-    <col min="4" max="4" width="24.28515625" style="8"/>
-    <col min="5" max="5" width="16.5703125" style="8"/>
-    <col min="6" max="6" width="10.85546875" style="8"/>
-    <col min="7" max="7" width="27.28515625" style="12"/>
+    <col min="1" max="1" width="2.85546875" style="7"/>
+    <col min="2" max="2" width="42" style="14"/>
+    <col min="3" max="3" width="18.7109375" style="7"/>
+    <col min="4" max="4" width="24.28515625" style="7"/>
+    <col min="5" max="5" width="16.5703125" style="7"/>
+    <col min="6" max="6" width="10.85546875" style="7"/>
+    <col min="7" max="7" width="27.28515625" style="11"/>
     <col min="8" max="1023" width="10.85546875"/>
     <col min="1024" max="1025" width="10.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>42433</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>42433</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="10"/>
+      <c r="G4" s="9"/>
     </row>
     <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>2</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>42453</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>42453</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>3</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>42453</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>42453</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>4</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>42453</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>42453</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>5</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>42453</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>42453</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+    <row r="9" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>6</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="11"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="B9" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="5">
+        <v>42461</v>
+      </c>
+      <c r="E9" s="5">
+        <v>42461</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>7</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="11"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="B10" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="5">
+        <v>42461</v>
+      </c>
+      <c r="E10" s="5">
+        <v>42461</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>8</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="11"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="B11" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="5">
+        <v>42461</v>
+      </c>
+      <c r="E11" s="5">
+        <v>42461</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
         <v>9</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="11"/>
+      <c r="B12" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="5">
+        <v>42461</v>
+      </c>
+      <c r="E12" s="5">
+        <v>42461</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="A13" s="2">
         <v>10</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="11"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="10"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+      <c r="A14" s="2">
         <v>11</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="11"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="10"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+      <c r="A15" s="2">
         <v>12</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="11"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="10"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+      <c r="A16" s="2">
         <v>13</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="11"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="10"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
+      <c r="A17" s="2">
         <v>14</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="11"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="10"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
+      <c r="A18" s="2">
         <v>15</v>
       </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="11"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="10"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+      <c r="A19" s="2">
         <v>16</v>
       </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="11"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="10"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+      <c r="A20" s="2">
         <v>17</v>
       </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="11"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="10"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
+      <c r="A21" s="2">
         <v>18</v>
       </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="11"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="10"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
+      <c r="A22" s="2">
         <v>19</v>
       </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="11"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="10"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
+      <c r="A23" s="2">
         <v>20</v>
       </c>
-      <c r="B23" s="14"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="11"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="10"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
+      <c r="A24" s="2">
         <v>21</v>
       </c>
-      <c r="B24" s="14"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="11"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="10"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
+      <c r="A25" s="2">
         <v>22</v>
       </c>
-      <c r="B25" s="14"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="11"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="10"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
+      <c r="A26" s="2">
         <v>23</v>
       </c>
-      <c r="B26" s="14"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="11"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="10"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
+      <c r="A27" s="2">
         <v>24</v>
       </c>
-      <c r="B27" s="14"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="11"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="10"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
+      <c r="A28" s="2">
         <v>25</v>
       </c>
-      <c r="B28" s="14"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="11"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Auditoria al monitoreo de las activiades del 8 al 14 de abril, 2016
</commit_message>
<xml_diff>
--- a/Proyectos/2016/Calidad/No_conformidades_organizacionales.xlsx
+++ b/Proyectos/2016/Calidad/No_conformidades_organizacionales.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="27">
   <si>
     <t>REPORTE DE NO CONFORMIDADES</t>
   </si>
@@ -95,6 +95,12 @@
   </si>
   <si>
     <t>Al no haber sido realizada la tarea no cuenta con registro de tiempo.</t>
+  </si>
+  <si>
+    <t>Las tareas atrasadas no cuentan con un comentario de seguimiento.</t>
+  </si>
+  <si>
+    <t>La actividade del 14 no tiene comentario.</t>
   </si>
 </sst>
 </file>
@@ -252,11 +258,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -611,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,24 +635,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -880,7 +886,7 @@
       <c r="A13" s="2">
         <v>10</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="15" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -903,7 +909,7 @@
       <c r="A14" s="2">
         <v>11</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="15" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -922,27 +928,51 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>12</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="10"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="5">
+        <v>42475</v>
+      </c>
+      <c r="E15" s="5">
+        <v>42475</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>13</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="10"/>
+      <c r="B16" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="5">
+        <v>42475</v>
+      </c>
+      <c r="E16" s="5">
+        <v>42475</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2">

</xml_diff>

<commit_message>
Auditoria al monitoreo de las activiades del 15 al 21 de abril, 2016
</commit_message>
<xml_diff>
--- a/Proyectos/2016/Calidad/No_conformidades_organizacionales.xlsx
+++ b/Proyectos/2016/Calidad/No_conformidades_organizacionales.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="No Conformidades" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="32">
   <si>
     <t>REPORTE DE NO CONFORMIDADES</t>
   </si>
@@ -101,6 +101,21 @@
   </si>
   <si>
     <t>La actividade del 14 no tiene comentario.</t>
+  </si>
+  <si>
+    <t>Algunas de las actividades retrasadas no cuentan con seguimiento.</t>
+  </si>
+  <si>
+    <t>La auditoria a procesos y productos no ha sido completada.</t>
+  </si>
+  <si>
+    <t>Calidad</t>
+  </si>
+  <si>
+    <t>La tarea de 20 y 21 no estan completadas.</t>
+  </si>
+  <si>
+    <t>Faltan algunas tareas por completar.</t>
   </si>
 </sst>
 </file>
@@ -617,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -974,49 +989,97 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>14</v>
       </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="10"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="5">
+        <v>42482</v>
+      </c>
+      <c r="E17" s="5">
+        <v>42482</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>15</v>
       </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="10"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="5">
+        <v>42482</v>
+      </c>
+      <c r="E18" s="5">
+        <v>42482</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>16</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="10"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="5">
+        <v>42482</v>
+      </c>
+      <c r="E19" s="5">
+        <v>42482</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>17</v>
       </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="10"/>
+      <c r="B20" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="5">
+        <v>42482</v>
+      </c>
+      <c r="E20" s="5">
+        <v>42482</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2">

</xml_diff>

<commit_message>
Monitoreo a las actividades del 22 al 29 de abril, 2016
</commit_message>
<xml_diff>
--- a/Proyectos/2016/Calidad/No_conformidades_organizacionales.xlsx
+++ b/Proyectos/2016/Calidad/No_conformidades_organizacionales.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="33">
   <si>
     <t>REPORTE DE NO CONFORMIDADES</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>Faltan algunas tareas por completar.</t>
+  </si>
+  <si>
+    <t>La actividad del 28 de abril no tiene comentarios</t>
   </si>
 </sst>
 </file>
@@ -632,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1081,27 +1084,51 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>18</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="10"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="5">
+        <v>42489</v>
+      </c>
+      <c r="E21" s="5">
+        <v>42489</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>19</v>
       </c>
-      <c r="B22" s="13"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="10"/>
+      <c r="B22" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="5">
+        <v>42489</v>
+      </c>
+      <c r="E22" s="5">
+        <v>42489</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2">

</xml_diff>

<commit_message>
Monitoreo a las actividades del 29 de abril al 6 de mayo
</commit_message>
<xml_diff>
--- a/Proyectos/2016/Calidad/No_conformidades_organizacionales.xlsx
+++ b/Proyectos/2016/Calidad/No_conformidades_organizacionales.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp EliteBook\Documents\Repositorio\SOSQTP\Proyectos\2016\Calidad\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shizel\Documents\SOSQTP\Proyectos\2016\Calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="35">
   <si>
     <t>REPORTE DE NO CONFORMIDADES</t>
   </si>
@@ -119,6 +119,12 @@
   </si>
   <si>
     <t>La actividad del 28 de abril no tiene comentarios</t>
+  </si>
+  <si>
+    <t>No todas las tareas se encontraban cronometradas</t>
+  </si>
+  <si>
+    <t>Las tareas no fueron completadas en su tiempo</t>
   </si>
 </sst>
 </file>
@@ -635,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26:G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1130,27 +1136,51 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>20</v>
       </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="10"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="5">
+        <v>42557</v>
+      </c>
+      <c r="E23" s="5">
+        <v>42557</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>21</v>
       </c>
-      <c r="B24" s="13"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="10"/>
+      <c r="B24" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="5">
+        <v>42557</v>
+      </c>
+      <c r="E24" s="5">
+        <v>42557</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
@@ -1158,10 +1188,10 @@
       </c>
       <c r="B25" s="13"/>
       <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
       <c r="F25" s="4"/>
-      <c r="G25" s="10"/>
+      <c r="G25" s="9"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
@@ -1169,10 +1199,10 @@
       </c>
       <c r="B26" s="13"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
       <c r="F26" s="4"/>
-      <c r="G26" s="10"/>
+      <c r="G26" s="9"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2">

</xml_diff>

<commit_message>
Monitoreo de las actividades del  6 al 13 de Mayo
</commit_message>
<xml_diff>
--- a/Proyectos/2016/Calidad/No_conformidades_organizacionales.xlsx
+++ b/Proyectos/2016/Calidad/No_conformidades_organizacionales.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="37">
   <si>
     <t>REPORTE DE NO CONFORMIDADES</t>
   </si>
@@ -125,6 +125,12 @@
   </si>
   <si>
     <t>Las tareas no fueron completadas en su tiempo</t>
+  </si>
+  <si>
+    <t>No todas las tareas tienen registro de tiempo</t>
+  </si>
+  <si>
+    <t>Las tareas no fueron realizadas</t>
   </si>
 </sst>
 </file>
@@ -641,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26:G28"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1147,10 +1153,10 @@
         <v>12</v>
       </c>
       <c r="D23" s="5">
-        <v>42557</v>
+        <v>42496</v>
       </c>
       <c r="E23" s="5">
-        <v>42557</v>
+        <v>42496</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>10</v>
@@ -1170,10 +1176,10 @@
         <v>18</v>
       </c>
       <c r="D24" s="5">
-        <v>42557</v>
+        <v>42496</v>
       </c>
       <c r="E24" s="5">
-        <v>42557</v>
+        <v>42496</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>10</v>
@@ -1182,27 +1188,51 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>22</v>
       </c>
-      <c r="B25" s="13"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="9"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="5">
+        <v>42503</v>
+      </c>
+      <c r="E25" s="5">
+        <v>42503</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>23</v>
       </c>
-      <c r="B26" s="13"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="9"/>
+      <c r="B26" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="5">
+        <v>42503</v>
+      </c>
+      <c r="E26" s="5">
+        <v>42503</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2">

</xml_diff>

<commit_message>
Monitoreo de las actividades del 13 al 20 de mayo
</commit_message>
<xml_diff>
--- a/Proyectos/2016/Calidad/No_conformidades_organizacionales.xlsx
+++ b/Proyectos/2016/Calidad/No_conformidades_organizacionales.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="37">
   <si>
     <t>REPORTE DE NO CONFORMIDADES</t>
   </si>
@@ -244,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -272,9 +272,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -647,42 +644,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" style="7"/>
-    <col min="2" max="2" width="42" style="14"/>
+    <col min="2" max="2" width="42" style="13"/>
     <col min="3" max="3" width="18.7109375" style="7"/>
     <col min="4" max="4" width="24.28515625" style="7"/>
     <col min="5" max="5" width="16.5703125" style="7"/>
     <col min="6" max="6" width="10.85546875" style="7"/>
-    <col min="7" max="7" width="27.28515625" style="11"/>
+    <col min="7" max="7" width="27.28515625" style="10"/>
     <col min="8" max="1023" width="10.85546875"/>
     <col min="1024" max="1025" width="10.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -711,7 +708,7 @@
       <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -732,7 +729,7 @@
       <c r="A5" s="2">
         <v>2</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -755,7 +752,7 @@
       <c r="A6" s="2">
         <v>3</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="12" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -778,7 +775,7 @@
       <c r="A7" s="2">
         <v>4</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -801,7 +798,7 @@
       <c r="A8" s="2">
         <v>5</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="12" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -824,7 +821,7 @@
       <c r="A9" s="2">
         <v>6</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -847,7 +844,7 @@
       <c r="A10" s="2">
         <v>7</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="12" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -870,7 +867,7 @@
       <c r="A11" s="2">
         <v>8</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="12" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -893,7 +890,7 @@
       <c r="A12" s="2">
         <v>9</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="12" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -916,7 +913,7 @@
       <c r="A13" s="2">
         <v>10</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="14" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -939,7 +936,7 @@
       <c r="A14" s="2">
         <v>11</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="14" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -962,7 +959,7 @@
       <c r="A15" s="2">
         <v>12</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="14" t="s">
         <v>25</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -985,7 +982,7 @@
       <c r="A16" s="2">
         <v>13</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="14" t="s">
         <v>26</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -1008,7 +1005,7 @@
       <c r="A17" s="2">
         <v>14</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="12" t="s">
         <v>27</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -1031,7 +1028,7 @@
       <c r="A18" s="2">
         <v>15</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="12" t="s">
         <v>28</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -1054,7 +1051,7 @@
       <c r="A19" s="2">
         <v>16</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="12" t="s">
         <v>30</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -1077,7 +1074,7 @@
       <c r="A20" s="2">
         <v>17</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="12" t="s">
         <v>31</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -1100,7 +1097,7 @@
       <c r="A21" s="2">
         <v>18</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="12" t="s">
         <v>27</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -1123,7 +1120,7 @@
       <c r="A22" s="2">
         <v>19</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="12" t="s">
         <v>32</v>
       </c>
       <c r="C22" s="2" t="s">
@@ -1146,7 +1143,7 @@
       <c r="A23" s="2">
         <v>20</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="12" t="s">
         <v>33</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -1169,7 +1166,7 @@
       <c r="A24" s="2">
         <v>21</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="12" t="s">
         <v>34</v>
       </c>
       <c r="C24" s="2" t="s">
@@ -1192,7 +1189,7 @@
       <c r="A25" s="2">
         <v>22</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="12" t="s">
         <v>35</v>
       </c>
       <c r="C25" s="2" t="s">
@@ -1215,7 +1212,7 @@
       <c r="A26" s="2">
         <v>23</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C26" s="2" t="s">
@@ -1234,27 +1231,51 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>24</v>
       </c>
-      <c r="B27" s="13"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="10"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="5">
+        <v>42510</v>
+      </c>
+      <c r="E27" s="5">
+        <v>42510</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>25</v>
       </c>
-      <c r="B28" s="13"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="10"/>
+      <c r="B28" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="5">
+        <v>42510</v>
+      </c>
+      <c r="E28" s="5">
+        <v>42510</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
La auditoría al Reporte de Monitoreo al mes de Abril 2016
</commit_message>
<xml_diff>
--- a/Proyectos/2016/Calidad/No_conformidades_organizacionales.xlsx
+++ b/Proyectos/2016/Calidad/No_conformidades_organizacionales.xlsx
@@ -5,21 +5,24 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shizel\Documents\SOSQTP\Proyectos\2016\Calidad\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Novela\Google Drive\1. Administración  Ci911 y SOS\2. SOS Software\10. CMMI\1. Auditoría Rep. Monitoreo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" tabRatio="989"/>
   </bookViews>
   <sheets>
     <sheet name="No Conformidades" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="41">
   <si>
     <t>REPORTE DE NO CONFORMIDADES</t>
   </si>
@@ -131,6 +134,18 @@
   </si>
   <si>
     <t>Las tareas no fueron realizadas</t>
+  </si>
+  <si>
+    <t>Se revisaron las acciones correctivas, pero no se analizaron si provenían de un riesgo. Una vez que se agregue se va a ver reflejado.</t>
+  </si>
+  <si>
+    <t>Reporte de Monitoreo</t>
+  </si>
+  <si>
+    <t>En proceso</t>
+  </si>
+  <si>
+    <t>Se reporta la falta de Análisis de riesgos al reporte de monitoreo.</t>
   </si>
 </sst>
 </file>
@@ -295,8 +310,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -380,7 +423,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -642,13 +685,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" style="7"/>
     <col min="2" max="2" width="42" style="13"/>
@@ -1277,12 +1320,46 @@
         <v>13</v>
       </c>
     </row>
+    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>26</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="5">
+        <v>42514</v>
+      </c>
+      <c r="E29" s="5">
+        <v>42527</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>27</v>
+      </c>
+      <c r="B30" s="12"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="9"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:G2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F28">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F30">
       <formula1>"En proceso,Cerrada,Cancelada,Rechazada"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Monitoreo de actividades del 20 al 27 de mayo
</commit_message>
<xml_diff>
--- a/Proyectos/2016/Calidad/No_conformidades_organizacionales.xlsx
+++ b/Proyectos/2016/Calidad/No_conformidades_organizacionales.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Novela\Google Drive\1. Administración  Ci911 y SOS\2. SOS Software\10. CMMI\1. Auditoría Rep. Monitoreo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shizel\Documents\SOSQTP\Proyectos\2016\Calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="42">
   <si>
     <t>REPORTE DE NO CONFORMIDADES</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t>Se reporta la falta de Análisis de riesgos al reporte de monitoreo.</t>
+  </si>
+  <si>
+    <t>No todas las tareas fueron realizadas</t>
   </si>
 </sst>
 </file>
@@ -423,7 +426,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -685,13 +688,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" style="7"/>
     <col min="2" max="2" width="42" style="13"/>
@@ -1343,23 +1346,58 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>27</v>
       </c>
-      <c r="B30" s="12"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="9"/>
+      <c r="B30" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="5">
+        <v>42517</v>
+      </c>
+      <c r="E30" s="5">
+        <v>42517</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>28</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="5">
+        <v>42517</v>
+      </c>
+      <c r="E31" s="5">
+        <v>42517</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:G2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F30">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F31">
       <formula1>"En proceso,Cerrada,Cancelada,Rechazada"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>